<commit_message>
Replaced kill with soft close app
</commit_message>
<xml_diff>
--- a/Data/Input/InputFile.xlsx
+++ b/Data/Input/InputFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\PoolCleansingPOC\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0066CBA7-9FCE-48D6-A75B-D689CBB3FB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90C68A4-162C-4CE6-86CD-B0A8C4A60CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -920,7 +920,7 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3717,7 +3717,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3821,7 +3821,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>21332229</v>
+        <v>21332355</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -3833,10 +3833,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -3848,7 +3848,7 @@
         <v>31</v>
       </c>
       <c r="M2" s="2">
-        <v>45159.380555555559</v>
+        <v>45159.386111111111</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added RetryScope for 'ClickRefresh' in 'ValidateEvent'
</commit_message>
<xml_diff>
--- a/Data/Input/InputFile.xlsx
+++ b/Data/Input/InputFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\PoolCleansingPOC\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90C68A4-162C-4CE6-86CD-B0A8C4A60CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A460D49-979D-4837-816F-FB7AF7A77BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="191">
   <si>
     <t>Action</t>
   </si>
@@ -593,6 +593,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>App Exception</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -917,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58164DE-A556-4979-84FE-E12BA5ED3B60}">
-  <dimension ref="A1:W49"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,7 +954,7 @@
     <col min="23" max="23" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>188</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>188</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>188</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>188</v>
       </c>
@@ -1243,7 +1249,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -1299,9 +1305,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B7">
         <v>21332355</v>
@@ -1355,9 +1361,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B8">
         <v>21332368</v>
@@ -1411,9 +1417,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>21332448</v>
@@ -1467,9 +1473,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B10">
         <v>21332484</v>
@@ -1522,10 +1528,13 @@
       <c r="W10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B11">
         <v>21332544</v>
@@ -1579,9 +1588,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <v>21332554</v>
@@ -1634,8 +1643,11 @@
       <c r="W12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1691,7 +1703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1747,7 +1759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1803,7 +1815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3714,10 +3726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE176C0-309D-433C-8DD4-9DA3971BC217}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3726,8 +3738,8 @@
     <col min="2" max="2" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
@@ -3821,7 +3833,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>21332355</v>
+        <v>21332368</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -3833,10 +3845,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -3848,7 +3860,7 @@
         <v>31</v>
       </c>
       <c r="M2" s="2">
-        <v>45159.386111111111</v>
+        <v>45159.386805555558</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -3869,6 +3881,286 @@
         <v>101</v>
       </c>
       <c r="W2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>21332448</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="2">
+        <v>45159.390277777777</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" t="s">
+        <v>101</v>
+      </c>
+      <c r="U3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" t="s">
+        <v>101</v>
+      </c>
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>21332484</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2">
+        <v>45159.39166666667</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" t="s">
+        <v>101</v>
+      </c>
+      <c r="U4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" t="s">
+        <v>101</v>
+      </c>
+      <c r="W4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>21332544</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="2">
+        <v>45159.394444444442</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>161</v>
+      </c>
+      <c r="S5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" t="s">
+        <v>36</v>
+      </c>
+      <c r="V5" t="s">
+        <v>101</v>
+      </c>
+      <c r="W5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>21332554</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="2">
+        <v>45159.395138888889</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" t="s">
+        <v>101</v>
+      </c>
+      <c r="U6" t="s">
+        <v>36</v>
+      </c>
+      <c r="V6" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>21332669</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="2">
+        <v>45159.399305555555</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" t="s">
+        <v>75</v>
+      </c>
+      <c r="S7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" t="s">
+        <v>101</v>
+      </c>
+      <c r="U7" t="s">
+        <v>36</v>
+      </c>
+      <c r="V7" t="s">
+        <v>101</v>
+      </c>
+      <c r="W7" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved 'KillAllApps' out of FirstRun, Added delay after transaction completion
</commit_message>
<xml_diff>
--- a/Data/Input/InputFile.xlsx
+++ b/Data/Input/InputFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\PoolCleansingPOC\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A460D49-979D-4837-816F-FB7AF7A77BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1644E829-BCD2-4FA5-978F-44934F1FDBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="193">
   <si>
     <t>Action</t>
   </si>
@@ -599,6 +599,12 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>No Records</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -925,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58164DE-A556-4979-84FE-E12BA5ED3B60}">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1649,7 +1655,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B13">
         <v>21332669</v>
@@ -1702,10 +1708,13 @@
       <c r="W13" t="s">
         <v>24</v>
       </c>
+      <c r="X13" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B14">
         <v>21332740</v>
@@ -1758,10 +1767,13 @@
       <c r="W14" t="s">
         <v>24</v>
       </c>
+      <c r="X14" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B15">
         <v>21332819</v>
@@ -1814,10 +1826,13 @@
       <c r="W15" t="s">
         <v>24</v>
       </c>
+      <c r="X15" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B16">
         <v>21333240</v>
@@ -1870,10 +1885,13 @@
       <c r="W16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B17">
         <v>21333905</v>
@@ -1926,10 +1944,13 @@
       <c r="W17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B18">
         <v>21334471</v>
@@ -1982,10 +2003,13 @@
       <c r="W18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B19">
         <v>21334792</v>
@@ -2039,9 +2063,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B20">
         <v>21336485</v>
@@ -2095,9 +2119,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B21">
         <v>21336785</v>
@@ -2151,9 +2175,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B22">
         <v>21337466</v>
@@ -2207,9 +2231,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B23">
         <v>21345638</v>
@@ -2263,9 +2287,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B24">
         <v>21346080</v>
@@ -2319,9 +2343,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B25">
         <v>21346170</v>
@@ -2375,7 +2399,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2431,7 +2455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2543,7 +2567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2599,7 +2623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2655,7 +2679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -2711,7 +2735,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -3726,10 +3750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE176C0-309D-433C-8DD4-9DA3971BC217}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3828,342 +3852,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>21332368</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="2">
-        <v>45159.386805555558</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>21332448</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="2">
-        <v>45159.390277777777</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" t="s">
-        <v>101</v>
-      </c>
-      <c r="U3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" t="s">
-        <v>101</v>
-      </c>
-      <c r="W3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>21332484</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>162</v>
-      </c>
-      <c r="G4" t="s">
-        <v>163</v>
-      </c>
-      <c r="H4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="2">
-        <v>45159.39166666667</v>
-      </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" t="s">
-        <v>101</v>
-      </c>
-      <c r="U4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" t="s">
-        <v>101</v>
-      </c>
-      <c r="W4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>21332544</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="2">
-        <v>45159.394444444442</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" t="s">
-        <v>161</v>
-      </c>
-      <c r="S5" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" t="s">
-        <v>101</v>
-      </c>
-      <c r="U5" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" t="s">
-        <v>101</v>
-      </c>
-      <c r="W5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>21332554</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" t="s">
-        <v>158</v>
-      </c>
-      <c r="H6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="2">
-        <v>45159.395138888889</v>
-      </c>
-      <c r="N6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" t="s">
-        <v>75</v>
-      </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" t="s">
-        <v>101</v>
-      </c>
-      <c r="U6" t="s">
-        <v>36</v>
-      </c>
-      <c r="V6" t="s">
-        <v>101</v>
-      </c>
-      <c r="W6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>21332669</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="2">
-        <v>45159.399305555555</v>
-      </c>
-      <c r="N7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" t="s">
-        <v>75</v>
-      </c>
-      <c r="S7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" t="s">
-        <v>101</v>
-      </c>
-      <c r="U7" t="s">
-        <v>36</v>
-      </c>
-      <c r="V7" t="s">
-        <v>101</v>
-      </c>
-      <c r="W7" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>